<commit_message>
input gain calculation for ADC
</commit_message>
<xml_diff>
--- a/Simulations/RCL Filter.xlsx
+++ b/Simulations/RCL Filter.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\UdeS_S7_APP1\Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA13E8EA-9C72-4608-912A-4AA7C10C3E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CA90C5-1A10-4F29-8C97-9D18C0A1E8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="5655" windowWidth="25440" windowHeight="15270" xr2:uid="{F6E68F60-B857-4FD9-B818-9D3C7F79BCB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F6E68F60-B857-4FD9-B818-9D3C7F79BCB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RCL" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>L</t>
   </si>
@@ -66,6 +67,30 @@
   </si>
   <si>
     <t>L_DCR</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Rf</t>
+  </si>
+  <si>
+    <t>Rg</t>
+  </si>
+  <si>
+    <t>Rin</t>
+  </si>
+  <si>
+    <t>Imp</t>
+  </si>
+  <si>
+    <t>Rt</t>
   </si>
 </sst>
 </file>
@@ -419,13 +444,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DD8B58-4CF3-4C74-B0B9-71C6587E5D4B}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -434,14 +461,14 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>49.9</v>
+        <v>10</v>
       </c>
       <c r="C1">
         <v>1</v>
       </c>
       <c r="D1">
         <f>C1 * B1</f>
-        <v>49.9</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -509,11 +536,11 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.72</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f>B4</f>
-        <v>0.72</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -539,10 +566,141 @@
       </c>
       <c r="B8">
         <f>1/(B1 + B4) * H2</f>
-        <v>0.23575983462657255</v>
+        <v>0.99451356906642507</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5C0E07-F387-43E9-A1AE-65552B2F3B96}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <f>B1/B2</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>B1 * B4 / B2</f>
+        <v>396</v>
+      </c>
+      <c r="D6">
+        <v>392</v>
+      </c>
+      <c r="E6">
+        <v>402</v>
+      </c>
+      <c r="F6">
+        <f>768 / 2</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>D6/$B$4</f>
+        <v>1.187878787878788</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:F7" si="0">E6/$B$4</f>
+        <v>1.2181818181818183</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.1636363636363636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>$B$2 * D7</f>
+        <v>2.9696969696969697</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:F8" si="1">$B$2 * E7</f>
+        <v>3.0454545454545459</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2.9090909090909092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <f>B4/(1-F6/(2*(B4+F6)))</f>
+        <v>451.37931034482756</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <f>1/ABS(1/B12-1/B11)</f>
+        <v>56.228522336769757</v>
+      </c>
+      <c r="D13">
+        <v>56.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f xml:space="preserve"> 1 / (1 / B11 + 1 / D13)</f>
+        <v>49.97744534572481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>